<commit_message>
Ajout JM Calculs V2
</commit_message>
<xml_diff>
--- a/Calculs/DataBase_template.xlsx
+++ b/Calculs/DataBase_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Citallios\Calculs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BA1E7C-B8FC-4355-9551-97ED2105A4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F8E57B-582A-4FA5-8F0B-748EB916CBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{8EF40DC6-95CA-4DEC-96C2-8670439CBDFF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="40">
   <si>
     <t>fck</t>
   </si>
@@ -95,9 +95,6 @@
     <t>m_els_2</t>
   </si>
   <si>
-    <t>m_elu</t>
-  </si>
-  <si>
     <t>m_feu</t>
   </si>
   <si>
@@ -150,6 +147,12 @@
   </si>
   <si>
     <t>File A - 3</t>
+  </si>
+  <si>
+    <t>m_elu_1</t>
+  </si>
+  <si>
+    <t>m_elu_2</t>
   </si>
 </sst>
 </file>
@@ -1017,20 +1020,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054D0C79-7D52-471E-B026-05BF71C3F576}">
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1093,24 +1096,27 @@
         <v>19</v>
       </c>
       <c r="W1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
       <c r="C2">
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>500</v>
@@ -1161,30 +1167,34 @@
         <v>1</v>
       </c>
       <c r="U2">
-        <v>38.13888</v>
+        <v>29.253119999999999</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>8.8857599999999994</v>
       </c>
       <c r="W2">
         <v>49.92</v>
       </c>
       <c r="X2">
+        <f>U2+V2</f>
         <v>38.13888</v>
       </c>
+      <c r="Y2">
+        <v>38.13888</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>500</v>
@@ -1235,30 +1245,34 @@
         <v>1</v>
       </c>
       <c r="U3">
-        <v>105.04999999999998</v>
+        <v>80.574999999999989</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>24.474999999999998</v>
       </c>
       <c r="W3">
         <v>137.5</v>
       </c>
       <c r="X3">
+        <f t="shared" ref="X3:X27" si="0">U3+V3</f>
         <v>105.04999999999998</v>
       </c>
+      <c r="Y3">
+        <v>105.04999999999998</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>500</v>
@@ -1309,30 +1323,34 @@
         <v>1</v>
       </c>
       <c r="U4">
-        <v>40.094720000000002</v>
+        <v>30.75328</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>9.3414400000000004</v>
       </c>
       <c r="W4">
         <v>52.480000000000004</v>
       </c>
       <c r="X4">
+        <f t="shared" si="0"/>
         <v>40.094720000000002</v>
       </c>
+      <c r="Y4">
+        <v>40.094720000000002</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>500</v>
@@ -1383,30 +1401,34 @@
         <v>1</v>
       </c>
       <c r="U5">
-        <v>75.63600000000001</v>
+        <v>58.014000000000003</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>17.622000000000003</v>
       </c>
       <c r="W5">
         <v>99.000000000000014</v>
       </c>
       <c r="X5">
+        <f t="shared" si="0"/>
         <v>75.63600000000001</v>
       </c>
+      <c r="Y5">
+        <v>75.63600000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>500</v>
@@ -1457,30 +1479,34 @@
         <v>1</v>
       </c>
       <c r="U6">
-        <v>39.116799999999998</v>
+        <v>30.0032</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>9.1135999999999999</v>
       </c>
       <c r="W6">
         <v>51.2</v>
       </c>
       <c r="X6">
+        <f t="shared" si="0"/>
         <v>39.116799999999998</v>
       </c>
+      <c r="Y6">
+        <v>39.116799999999998</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>500</v>
@@ -1531,30 +1557,34 @@
         <v>1</v>
       </c>
       <c r="U7">
-        <v>126.06</v>
+        <v>96.69</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>29.369999999999997</v>
       </c>
       <c r="W7">
         <v>165</v>
       </c>
       <c r="X7">
+        <f t="shared" si="0"/>
         <v>126.06</v>
       </c>
+      <c r="Y7">
+        <v>126.06</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>500</v>
@@ -1605,30 +1635,34 @@
         <v>1</v>
       </c>
       <c r="U8">
-        <v>68.454400000000007</v>
+        <v>52.505600000000001</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>15.9488</v>
       </c>
       <c r="W8">
         <v>89.600000000000009</v>
       </c>
       <c r="X8">
+        <f t="shared" si="0"/>
         <v>68.454400000000007</v>
       </c>
+      <c r="Y8">
+        <v>68.454400000000007</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>500</v>
@@ -1679,30 +1713,34 @@
         <v>1</v>
       </c>
       <c r="U9">
-        <v>92.444000000000003</v>
+        <v>70.906000000000006</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>21.538</v>
       </c>
       <c r="W9">
         <v>121.00000000000001</v>
       </c>
       <c r="X9">
+        <f t="shared" si="0"/>
         <v>92.444000000000003</v>
       </c>
+      <c r="Y9">
+        <v>92.444000000000003</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10">
         <v>500</v>
@@ -1753,30 +1791,34 @@
         <v>1</v>
       </c>
       <c r="U10">
-        <v>7.6277759999999999</v>
+        <v>5.8506239999999998</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>1.7771519999999998</v>
       </c>
       <c r="W10">
         <v>9.984</v>
       </c>
       <c r="X10">
+        <f t="shared" si="0"/>
         <v>7.6277759999999999</v>
       </c>
+      <c r="Y10">
+        <v>7.6277759999999999</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11">
         <v>500</v>
@@ -1827,30 +1869,34 @@
         <v>1</v>
       </c>
       <c r="U11">
-        <v>25.211999999999996</v>
+        <v>19.337999999999997</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>5.8739999999999997</v>
       </c>
       <c r="W11">
         <v>33</v>
       </c>
       <c r="X11">
+        <f t="shared" si="0"/>
         <v>25.211999999999996</v>
       </c>
+      <c r="Y11">
+        <v>25.211999999999996</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>500</v>
@@ -1901,30 +1947,34 @@
         <v>1</v>
       </c>
       <c r="U12">
-        <v>8.8012799999999984</v>
+        <v>6.7507199999999994</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>2.0505599999999999</v>
       </c>
       <c r="W12">
         <v>11.52</v>
       </c>
       <c r="X12">
+        <f t="shared" si="0"/>
         <v>8.8012799999999984</v>
       </c>
+      <c r="Y12">
+        <v>8.8012799999999984</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>500</v>
@@ -1975,30 +2025,34 @@
         <v>1</v>
       </c>
       <c r="U13">
-        <v>92.444000000000003</v>
+        <v>70.906000000000006</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>21.538</v>
       </c>
       <c r="W13">
         <v>121.00000000000001</v>
       </c>
       <c r="X13">
+        <f t="shared" si="0"/>
         <v>92.444000000000003</v>
       </c>
+      <c r="Y13">
+        <v>92.444000000000003</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>500</v>
@@ -2049,30 +2103,34 @@
         <v>1</v>
       </c>
       <c r="U14">
-        <v>55.741440000000004</v>
+        <v>42.754560000000005</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>12.986880000000001</v>
       </c>
       <c r="W14">
         <v>72.960000000000008</v>
       </c>
       <c r="X14">
+        <f t="shared" si="0"/>
         <v>55.741440000000004</v>
       </c>
+      <c r="Y14">
+        <v>55.741440000000004</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15">
         <v>500</v>
@@ -2123,30 +2181,34 @@
         <v>1</v>
       </c>
       <c r="U15">
-        <v>121.858</v>
+        <v>93.466999999999999</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>28.390999999999998</v>
       </c>
       <c r="W15">
         <v>159.5</v>
       </c>
       <c r="X15">
+        <f t="shared" si="0"/>
         <v>121.858</v>
       </c>
+      <c r="Y15">
+        <v>121.858</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16">
         <v>500</v>
@@ -2197,30 +2259,34 @@
         <v>1</v>
       </c>
       <c r="U16">
-        <v>44.006399999999999</v>
+        <v>33.753599999999999</v>
       </c>
       <c r="V16">
-        <v>0</v>
+        <v>10.252800000000001</v>
       </c>
       <c r="W16">
         <v>57.6</v>
       </c>
       <c r="X16">
+        <f t="shared" si="0"/>
         <v>44.006399999999999</v>
       </c>
+      <c r="Y16">
+        <v>44.006399999999999</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17">
         <v>500</v>
@@ -2271,30 +2337,34 @@
         <v>1</v>
       </c>
       <c r="U17">
-        <v>36.183039999999998</v>
+        <v>27.752959999999998</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <v>8.4300800000000002</v>
       </c>
       <c r="W17">
         <v>47.36</v>
       </c>
       <c r="X17">
+        <f t="shared" si="0"/>
         <v>36.183039999999998</v>
       </c>
+      <c r="Y17">
+        <v>36.183039999999998</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18">
         <v>500</v>
@@ -2345,30 +2415,34 @@
         <v>1</v>
       </c>
       <c r="U18">
-        <v>126.06</v>
+        <v>96.69</v>
       </c>
       <c r="V18">
-        <v>0</v>
+        <v>29.369999999999997</v>
       </c>
       <c r="W18">
         <v>165</v>
       </c>
       <c r="X18">
+        <f t="shared" si="0"/>
         <v>126.06</v>
       </c>
+      <c r="Y18">
+        <v>126.06</v>
+      </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19">
         <v>500</v>
@@ -2419,30 +2493,34 @@
         <v>1</v>
       </c>
       <c r="U19">
-        <v>73.343999999999994</v>
+        <v>56.256</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>17.088000000000001</v>
       </c>
       <c r="W19">
         <v>96</v>
       </c>
       <c r="X19">
+        <f t="shared" si="0"/>
         <v>73.343999999999994</v>
       </c>
+      <c r="Y19">
+        <v>73.343999999999994</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20">
         <v>500</v>
@@ -2493,30 +2571,34 @@
         <v>1</v>
       </c>
       <c r="U20">
-        <v>92.444000000000003</v>
+        <v>70.906000000000006</v>
       </c>
       <c r="V20">
-        <v>0</v>
+        <v>21.538</v>
       </c>
       <c r="W20">
         <v>121.00000000000001</v>
       </c>
       <c r="X20">
+        <f t="shared" si="0"/>
         <v>92.444000000000003</v>
       </c>
+      <c r="Y20">
+        <v>92.444000000000003</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21">
         <v>500</v>
@@ -2567,30 +2649,34 @@
         <v>1</v>
       </c>
       <c r="U21">
-        <v>2.7381759999999997</v>
+        <v>2.1002239999999999</v>
       </c>
       <c r="V21">
-        <v>0</v>
+        <v>0.63795199999999985</v>
       </c>
       <c r="W21">
         <v>3.5839999999999996</v>
       </c>
       <c r="X21">
+        <f t="shared" si="0"/>
         <v>2.7381759999999997</v>
       </c>
+      <c r="Y21">
+        <v>2.7381759999999997</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E22">
         <v>500</v>
@@ -2641,30 +2727,34 @@
         <v>1</v>
       </c>
       <c r="U22">
+        <v>19.337999999999997</v>
+      </c>
+      <c r="V22">
+        <v>5.8739999999999997</v>
+      </c>
+      <c r="W22">
+        <v>190</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="0"/>
         <v>25.211999999999996</v>
       </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22">
-        <v>33</v>
-      </c>
-      <c r="X22">
+      <c r="Y22">
         <v>25.211999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23">
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E23">
         <v>500</v>
@@ -2715,30 +2805,34 @@
         <v>1</v>
       </c>
       <c r="U23">
-        <v>7.4321919999999997</v>
+        <v>5.7006079999999999</v>
       </c>
       <c r="V23">
-        <v>0</v>
+        <v>1.7315839999999998</v>
       </c>
       <c r="W23">
         <v>9.7279999999999998</v>
       </c>
       <c r="X23">
+        <f t="shared" si="0"/>
         <v>7.4321919999999997</v>
       </c>
+      <c r="Y23">
+        <v>7.4321919999999997</v>
+      </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E24">
         <v>500</v>
@@ -2789,30 +2883,34 @@
         <v>1</v>
       </c>
       <c r="U24">
-        <v>92.444000000000003</v>
+        <v>70.906000000000006</v>
       </c>
       <c r="V24">
-        <v>0</v>
+        <v>21.538</v>
       </c>
       <c r="W24">
         <v>121.00000000000001</v>
       </c>
       <c r="X24">
+        <f t="shared" si="0"/>
         <v>92.444000000000003</v>
       </c>
+      <c r="Y24">
+        <v>92.444000000000003</v>
+      </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25">
         <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E25">
         <v>500</v>
@@ -2863,30 +2961,34 @@
         <v>1</v>
       </c>
       <c r="U25">
-        <v>73.343999999999994</v>
+        <v>56.256</v>
       </c>
       <c r="V25">
-        <v>0</v>
+        <v>17.088000000000001</v>
       </c>
       <c r="W25">
         <v>96</v>
       </c>
       <c r="X25">
+        <f t="shared" si="0"/>
         <v>73.343999999999994</v>
       </c>
+      <c r="Y25">
+        <v>73.343999999999994</v>
+      </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E26">
         <v>500</v>
@@ -2937,30 +3039,34 @@
         <v>1</v>
       </c>
       <c r="U26">
-        <v>121.858</v>
+        <v>93.466999999999999</v>
       </c>
       <c r="V26">
-        <v>0</v>
+        <v>28.390999999999998</v>
       </c>
       <c r="W26">
         <v>159.5</v>
       </c>
       <c r="X26">
+        <f t="shared" si="0"/>
         <v>121.858</v>
       </c>
+      <c r="Y26">
+        <v>121.858</v>
+      </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E27">
         <v>500</v>
@@ -3011,15 +3117,19 @@
         <v>1</v>
       </c>
       <c r="U27">
-        <v>36.183039999999998</v>
+        <v>27.752959999999998</v>
       </c>
       <c r="V27">
-        <v>0</v>
+        <v>8.4300800000000002</v>
       </c>
       <c r="W27">
         <v>47.36</v>
       </c>
       <c r="X27">
+        <f t="shared" si="0"/>
+        <v>36.183039999999998</v>
+      </c>
+      <c r="Y27">
         <v>36.183039999999998</v>
       </c>
     </row>

</xml_diff>